<commit_message>
In flight C.g. locations are done
</commit_message>
<xml_diff>
--- a/Measurement Analysis/Flight Data.xlsx
+++ b/Measurement Analysis/Flight Data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarta\OneDrive\Desktop\FlightDynamicsSVV\Measurement Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A5394E-4427-46C9-9FB9-54F4161B2F0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89490E0E-E1A2-47B7-9F6E-A91FFBF8F278}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight Data" sheetId="1" r:id="rId1"/>
     <sheet name="Weigjt&amp;Balance" sheetId="2" r:id="rId2"/>
+    <sheet name="Changing CG" sheetId="3" r:id="rId3"/>
+    <sheet name="Shifted CG Weight and Balance" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="109">
   <si>
     <t>Post-Flight Data Sheet AE3202</t>
   </si>
@@ -331,6 +333,54 @@
       <t xml:space="preserve"> [inches]</t>
     </r>
   </si>
+  <si>
+    <t>Measurement nr.</t>
+  </si>
+  <si>
+    <t>F.Used</t>
+  </si>
+  <si>
+    <t>Fremaining</t>
+  </si>
+  <si>
+    <t>Fremaining upper</t>
+  </si>
+  <si>
+    <t>Fremaining lower</t>
+  </si>
+  <si>
+    <t>Fmoment upper</t>
+  </si>
+  <si>
+    <t>Fmoment lower</t>
+  </si>
+  <si>
+    <t>Fmoment rem</t>
+  </si>
+  <si>
+    <t>Xc.g in flight (inches)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trim Curve </t>
+  </si>
+  <si>
+    <t>Shifted CG</t>
+  </si>
+  <si>
+    <t>Measurement nr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fremaining </t>
+  </si>
+  <si>
+    <t>xlemac</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>Xc.g [MAC]</t>
+  </si>
 </sst>
 </file>
 
@@ -339,7 +389,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +433,15 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -432,7 +491,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -453,14 +512,13 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -475,11 +533,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1559,7 +1619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M84"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
@@ -2970,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6141737-6818-4B76-A9F7-A606D8A3676F}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2987,62 +3047,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="9" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -3058,12 +3118,12 @@
         <f t="shared" ref="D5:D13" si="0">B5*C5</f>
         <v>10480</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
@@ -3079,10 +3139,10 @@
         <f t="shared" si="0"/>
         <v>13362</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -3098,16 +3158,16 @@
         <f t="shared" si="0"/>
         <v>17334</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="10">
         <v>291.64999999999998</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="10">
         <v>9165</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="10">
         <f>G7*F7</f>
         <v>2672972.25</v>
       </c>
@@ -3126,10 +3186,10 @@
         <f t="shared" si="0"/>
         <v>14124</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -3145,12 +3205,12 @@
         <f t="shared" si="0"/>
         <v>24849</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
@@ -3166,10 +3226,10 @@
         <f t="shared" si="0"/>
         <v>16064</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
@@ -3185,13 +3245,13 @@
         <f t="shared" si="0"/>
         <v>23328</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13">
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14">
         <f>C19</f>
         <v>760</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="14">
         <f>D19</f>
         <v>163013</v>
       </c>
@@ -3210,10 +3270,10 @@
         <f t="shared" si="0"/>
         <v>28512</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
@@ -3229,42 +3289,42 @@
         <f t="shared" si="0"/>
         <v>14960</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="9" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="11">
         <f>H15/G15</f>
         <v>285.74158690176324</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="10">
         <f>G7+G11</f>
         <v>9925</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="10">
         <f>H11+H7</f>
         <v>2835985.25</v>
       </c>
@@ -3282,10 +3342,10 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="E16" s="9"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
@@ -3300,12 +3360,12 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
@@ -3317,76 +3377,1019 @@
       <c r="D18">
         <v>0</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18">
+      <c r="B19" s="9"/>
+      <c r="C19" s="9">
         <f>SUM(C5:C13)+SUM(C16:C18)</f>
         <v>760</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="9">
         <f>SUM(D5:D13)+SUM(D16:D18)</f>
         <v>163013</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13">
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="14">
         <v>4100</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="14">
         <f>11705.5*100</f>
         <v>1170550</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E23" s="9" t="s">
+      <c r="E23" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="11">
         <f>H23/G23</f>
         <v>285.67096256684493</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="10">
         <f>G15+G19</f>
         <v>14025</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="10">
         <f>H19+H15</f>
         <v>4006535.25</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E24" s="9"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="E9:H10"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:H2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="E5:H6"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="A14:D15"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="E13:H14"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="E17:H18"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="E21:H22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C39D154-1F26-4105-A8FA-B8B6FE50AD62}">
+  <dimension ref="A1:J19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1">
+        <v>251.56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>80.98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <f>'Flight Data'!L59</f>
+        <v>778</v>
+      </c>
+      <c r="C8">
+        <f>'Weigjt&amp;Balance'!G$19-B8</f>
+        <v>3322</v>
+      </c>
+      <c r="D8">
+        <v>3400</v>
+      </c>
+      <c r="E8">
+        <f>D8-100</f>
+        <v>3300</v>
+      </c>
+      <c r="F8">
+        <f>9696.97*100</f>
+        <v>969696.99999999988</v>
+      </c>
+      <c r="G8">
+        <f>F10</f>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="H8">
+        <f>((F8-G8)/(D8-E8))*(C8-E8)+G8</f>
+        <v>925067.73999999987</v>
+      </c>
+      <c r="I8">
+        <f>('Weigjt&amp;Balance'!H$15+H8)/('Weigjt&amp;Balance'!G$15+'Changing CG'!C8)</f>
+        <v>283.91733902015551</v>
+      </c>
+      <c r="J8">
+        <f>(I8-B$1)/B$2</f>
+        <v>0.39957198098487906</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f>A8+1</f>
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <f>'Flight Data'!L60</f>
+        <v>797</v>
+      </c>
+      <c r="C9">
+        <f>'Weigjt&amp;Balance'!G$19-B9</f>
+        <v>3303</v>
+      </c>
+      <c r="D9">
+        <v>3400</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9:E14" si="0">D9-100</f>
+        <v>3300</v>
+      </c>
+      <c r="F9">
+        <f>9696.97*100</f>
+        <v>969696.99999999988</v>
+      </c>
+      <c r="G9">
+        <f>F11</f>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ref="H9:H19" si="1">((F9-G9)/(D9-E9))*(C9-E9)+G9</f>
+        <v>914196.50999999989</v>
+      </c>
+      <c r="I9">
+        <f>('Weigjt&amp;Balance'!H$15+H9)/('Weigjt&amp;Balance'!G$15+'Changing CG'!C9)</f>
+        <v>283.50330813426064</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ref="J9:J14" si="2">(I9-B$1)/B$2</f>
+        <v>0.39445922615782453</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" ref="A10:A14" si="3">A9+1</f>
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <f>'Flight Data'!L61</f>
+        <v>826</v>
+      </c>
+      <c r="C10">
+        <f>'Weigjt&amp;Balance'!G$19-B10</f>
+        <v>3274</v>
+      </c>
+      <c r="D10">
+        <v>3300</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="F10">
+        <f>9124.8*100</f>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="G10">
+        <f>8839.04*100</f>
+        <v>883904.00000000012</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>905050.24</v>
+      </c>
+      <c r="I10">
+        <f>('Weigjt&amp;Balance'!H$15+H10)/('Weigjt&amp;Balance'!G$15+'Changing CG'!C10)</f>
+        <v>283.4332517614971</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0.39359411906022596</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <f>'Flight Data'!L62</f>
+        <v>839</v>
+      </c>
+      <c r="C11">
+        <f>'Weigjt&amp;Balance'!G$19-B11</f>
+        <v>3261</v>
+      </c>
+      <c r="D11">
+        <v>3300</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F14" si="4">9124.8*100</f>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G14" si="5">8839.04*100</f>
+        <v>883904.00000000012</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>901335.36</v>
+      </c>
+      <c r="I11">
+        <f>('Weigjt&amp;Balance'!H$15+H11)/('Weigjt&amp;Balance'!G$15+'Changing CG'!C11)</f>
+        <v>283.43095783406642</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0.39356579197414687</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <f>'Flight Data'!L63</f>
+        <v>857</v>
+      </c>
+      <c r="C12">
+        <f>'Weigjt&amp;Balance'!G$19-B12</f>
+        <v>3243</v>
+      </c>
+      <c r="D12">
+        <v>3300</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="4"/>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="5"/>
+        <v>883904.00000000012</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>896191.68</v>
+      </c>
+      <c r="I12">
+        <f>('Weigjt&amp;Balance'!H$15+H12)/('Weigjt&amp;Balance'!G$15+'Changing CG'!C12)</f>
+        <v>283.42777414945323</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0.3935264775185629</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <f>'Flight Data'!L64</f>
+        <v>872</v>
+      </c>
+      <c r="C13">
+        <f>'Weigjt&amp;Balance'!G$19-B13</f>
+        <v>3228</v>
+      </c>
+      <c r="D13">
+        <v>3300</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="4"/>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>883904.00000000012</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>891905.28</v>
+      </c>
+      <c r="I13">
+        <f>('Weigjt&amp;Balance'!H$15+H13)/('Weigjt&amp;Balance'!G$15+'Changing CG'!C13)</f>
+        <v>283.42511442256523</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>0.39349363327445325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <f>'Flight Data'!L65</f>
+        <v>889</v>
+      </c>
+      <c r="C14">
+        <f>'Weigjt&amp;Balance'!G$19-B14</f>
+        <v>3211</v>
+      </c>
+      <c r="D14">
+        <v>3300</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>3200</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>883904.00000000012</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>887047.3600000001</v>
+      </c>
+      <c r="I14">
+        <f>('Weigjt&amp;Balance'!H$15+H14)/('Weigjt&amp;Balance'!G$15+'Changing CG'!C14)</f>
+        <v>283.4220927222899</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0.39345631911941098</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" t="s">
+        <v>101</v>
+      </c>
+      <c r="J17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f>'Flight Data'!L75</f>
+        <v>912</v>
+      </c>
+      <c r="C18">
+        <f>'Shifted CG Weight and Balance'!G$19-'Changing CG'!B18</f>
+        <v>3188</v>
+      </c>
+      <c r="D18">
+        <v>3200</v>
+      </c>
+      <c r="E18">
+        <v>3100</v>
+      </c>
+      <c r="F18">
+        <f>9124.8*100</f>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="G18">
+        <f>8839.04*100</f>
+        <v>883904.00000000012</v>
+      </c>
+      <c r="H18">
+        <f>((F18-G18)/(D18-E18))*(C18-E18)+G18</f>
+        <v>909050.87999999989</v>
+      </c>
+      <c r="I18">
+        <f>('Shifted CG Weight and Balance'!H$15+'Changing CG'!H18)/('Shifted CG Weight and Balance'!G$15+'Changing CG'!C18)</f>
+        <v>284.55533668878212</v>
+      </c>
+      <c r="J18">
+        <f>(I18-B$1)/B$2</f>
+        <v>0.4074504407110659</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <f>'Flight Data'!L76</f>
+        <v>944</v>
+      </c>
+      <c r="C19">
+        <f>'Shifted CG Weight and Balance'!G$19-'Changing CG'!B19</f>
+        <v>3156</v>
+      </c>
+      <c r="D19">
+        <v>3200</v>
+      </c>
+      <c r="E19">
+        <v>3100</v>
+      </c>
+      <c r="F19">
+        <f>9124.8*100</f>
+        <v>912479.99999999988</v>
+      </c>
+      <c r="G19">
+        <f>8839.04*100</f>
+        <v>883904.00000000012</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>899906.55999999994</v>
+      </c>
+      <c r="I19">
+        <f>('Shifted CG Weight and Balance'!H$15+'Changing CG'!H19)/('Shifted CG Weight and Balance'!G$15+'Changing CG'!C19)</f>
+        <v>284.55238972555617</v>
+      </c>
+      <c r="J19">
+        <f>(I19-B$1)/B$2</f>
+        <v>0.40741404946352389</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C0FC19-7574-4CE4-850E-55A2B515E3A9}">
+  <dimension ref="A1:H24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="5">
+        <v>131</v>
+      </c>
+      <c r="C5" s="5">
+        <v>80</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" ref="D5:D13" si="0">B5*C5</f>
+        <v>10480</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" s="5">
+        <v>131</v>
+      </c>
+      <c r="C6" s="5">
+        <v>102</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>13362</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="5">
+        <v>214</v>
+      </c>
+      <c r="C7" s="5">
+        <v>81</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>17334</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="10">
+        <v>291.64999999999998</v>
+      </c>
+      <c r="G7" s="10">
+        <v>9165</v>
+      </c>
+      <c r="H7" s="10">
+        <f>G7*F7</f>
+        <v>2672972.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="5">
+        <v>214</v>
+      </c>
+      <c r="C8" s="5">
+        <v>66</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>14124</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="5">
+        <v>251</v>
+      </c>
+      <c r="C9" s="5">
+        <v>99</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>24849</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="5">
+        <v>251</v>
+      </c>
+      <c r="C10" s="5">
+        <v>64</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>16064</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="5">
+        <v>288</v>
+      </c>
+      <c r="C11" s="5">
+        <v>81</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>23328</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14">
+        <f>C19</f>
+        <v>760</v>
+      </c>
+      <c r="H11" s="14">
+        <f>D19</f>
+        <v>149351</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="5">
+        <v>150</v>
+      </c>
+      <c r="C12" s="5">
+        <v>99</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>14850</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="5">
+        <v>170</v>
+      </c>
+      <c r="C13" s="5">
+        <v>88</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>14960</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="11">
+        <f>H15/G15</f>
+        <v>284.36506297229221</v>
+      </c>
+      <c r="G15" s="10">
+        <f>G7+G11</f>
+        <v>9925</v>
+      </c>
+      <c r="H15" s="10">
+        <f>H11+H7</f>
+        <v>2822323.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="5">
+        <v>74</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" s="5">
+        <v>321</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="5">
+        <v>338</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9">
+        <f>SUM(C5:C13)+SUM(C16:C18)</f>
+        <v>760</v>
+      </c>
+      <c r="D19" s="9">
+        <f>SUM(D5:D13)+SUM(D16:D18)</f>
+        <v>149351</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="14">
+        <v>4100</v>
+      </c>
+      <c r="H19" s="14">
+        <f>11705.5*100</f>
+        <v>1170550</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E23" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" s="11">
+        <f>H23/G23</f>
+        <v>284.69684491978609</v>
+      </c>
+      <c r="G23" s="10">
+        <f>G15+G19</f>
+        <v>14025</v>
+      </c>
+      <c r="H23" s="10">
+        <f>H19+H15</f>
+        <v>3992873.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E24" s="10"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="35">

</xml_diff>